<commit_message>
shifting fixed & color coding done
</commit_message>
<xml_diff>
--- a/data/projects_mapping/mwi_admin3_nso_points.xlsx
+++ b/data/projects_mapping/mwi_admin3_nso_points.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$434</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1533,7 +1536,28 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1719,7 +1743,7 @@
   <dimension ref="A1:E434"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4887,10 +4911,10 @@
         <v>202</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>33.0646073671507</v>
+        <v>33.092603</v>
       </c>
       <c r="E186" s="3" t="n">
-        <v>-9.52418902166024</v>
+        <v>-9.5692058</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9110,6 +9134,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E434"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -9117,5 +9142,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>